<commit_message>
bug fixes in the code and ensure reproducibility
</commit_message>
<xml_diff>
--- a/processed_data/Matrices_Stations.xlsx
+++ b/processed_data/Matrices_Stations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Afstand_km" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Duur_minuten" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Afstand_km" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Duur_minuten" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -698,7 +698,7 @@
         <v>112.18</v>
       </c>
       <c r="D6" t="n">
-        <v>139.87</v>
+        <v>135.64</v>
       </c>
       <c r="E6" t="n">
         <v>89.81</v>
@@ -728,7 +728,7 @@
         <v>87.95</v>
       </c>
       <c r="N6" t="n">
-        <v>126.49</v>
+        <v>126.38</v>
       </c>
     </row>
     <row r="7">
@@ -744,7 +744,7 @@
         <v>80.28</v>
       </c>
       <c r="D7" t="n">
-        <v>107.96</v>
+        <v>103.74</v>
       </c>
       <c r="E7" t="n">
         <v>82.95</v>
@@ -774,7 +774,7 @@
         <v>127.82</v>
       </c>
       <c r="N7" t="n">
-        <v>94.58</v>
+        <v>94.47</v>
       </c>
     </row>
     <row r="8">
@@ -882,7 +882,7 @@
         <v>50.35</v>
       </c>
       <c r="D10" t="n">
-        <v>78.03</v>
+        <v>73.81</v>
       </c>
       <c r="E10" t="n">
         <v>72.05</v>
@@ -897,7 +897,7 @@
         <v>106.1</v>
       </c>
       <c r="I10" t="n">
-        <v>254.75</v>
+        <v>254.74</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -912,7 +912,7 @@
         <v>148.22</v>
       </c>
       <c r="N10" t="n">
-        <v>64.65000000000001</v>
+        <v>64.54000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -928,7 +928,7 @@
         <v>117.42</v>
       </c>
       <c r="D11" t="n">
-        <v>140.91</v>
+        <v>140.88</v>
       </c>
       <c r="E11" t="n">
         <v>89.45</v>
@@ -958,7 +958,7 @@
         <v>139.89</v>
       </c>
       <c r="N11" t="n">
-        <v>131.73</v>
+        <v>131.62</v>
       </c>
     </row>
     <row r="12">
@@ -1017,10 +1017,10 @@
         <v>217.54</v>
       </c>
       <c r="C13" t="n">
-        <v>218.85</v>
+        <v>218.8</v>
       </c>
       <c r="D13" t="n">
-        <v>246.53</v>
+        <v>242.26</v>
       </c>
       <c r="E13" t="n">
         <v>177.67</v>
@@ -1035,7 +1035,7 @@
         <v>211.91</v>
       </c>
       <c r="I13" t="n">
-        <v>399.41</v>
+        <v>399.42</v>
       </c>
       <c r="J13" t="n">
         <v>147.84</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>233.15</v>
+        <v>232.99</v>
       </c>
     </row>
     <row r="14">
@@ -1213,7 +1213,7 @@
         <v>1971.07</v>
       </c>
       <c r="I2" t="n">
-        <v>8165.03</v>
+        <v>8165</v>
       </c>
       <c r="J2" t="n">
         <v>5255.44</v>
@@ -1238,13 +1238,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4095.65</v>
+        <v>4105.97</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>1626.28</v>
+        <v>1640.87</v>
       </c>
       <c r="E3" t="n">
         <v>3028.4</v>
@@ -1259,7 +1259,7 @@
         <v>4582.65</v>
       </c>
       <c r="I3" t="n">
-        <v>10752.55</v>
+        <v>10752.52</v>
       </c>
       <c r="J3" t="n">
         <v>3045.46</v>
@@ -1268,13 +1268,13 @@
         <v>5721.76</v>
       </c>
       <c r="L3" t="n">
-        <v>9136.040000000001</v>
+        <v>9150.639999999999</v>
       </c>
       <c r="M3" t="n">
         <v>8917.700000000001</v>
       </c>
       <c r="N3" t="n">
-        <v>1105.12</v>
+        <v>1119.72</v>
       </c>
     </row>
     <row r="4">
@@ -1284,7 +1284,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3285.37</v>
+        <v>3281.09</v>
       </c>
       <c r="C4" t="n">
         <v>1553.31</v>
@@ -1305,7 +1305,7 @@
         <v>3900.56</v>
       </c>
       <c r="I4" t="n">
-        <v>10094.53</v>
+        <v>10094.5</v>
       </c>
       <c r="J4" t="n">
         <v>3679.89</v>
@@ -1330,7 +1330,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2547.53</v>
+        <v>2543.26</v>
       </c>
       <c r="C5" t="n">
         <v>2999.04</v>
@@ -1351,7 +1351,7 @@
         <v>2498.39</v>
       </c>
       <c r="I5" t="n">
-        <v>8668.290000000001</v>
+        <v>8668.26</v>
       </c>
       <c r="J5" t="n">
         <v>3596.53</v>
@@ -1376,13 +1376,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6059.02</v>
+        <v>6054.75</v>
       </c>
       <c r="C6" t="n">
         <v>5538.57</v>
       </c>
       <c r="D6" t="n">
-        <v>6414.98</v>
+        <v>6268.44</v>
       </c>
       <c r="E6" t="n">
         <v>4427.29</v>
@@ -1412,7 +1412,7 @@
         <v>4527.86</v>
       </c>
       <c r="N6" t="n">
-        <v>6065.56</v>
+        <v>5747.29</v>
       </c>
     </row>
     <row r="7">
@@ -1422,19 +1422,19 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5745.01</v>
+        <v>5740.73</v>
       </c>
       <c r="C7" t="n">
-        <v>4077.48</v>
+        <v>4072.27</v>
       </c>
       <c r="D7" t="n">
-        <v>4953.88</v>
+        <v>4802.14</v>
       </c>
       <c r="E7" t="n">
         <v>4113.28</v>
       </c>
       <c r="F7" t="n">
-        <v>2775.11</v>
+        <v>2769.91</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1443,10 +1443,10 @@
         <v>5421.8</v>
       </c>
       <c r="I7" t="n">
-        <v>11591.7</v>
+        <v>11591.67</v>
       </c>
       <c r="J7" t="n">
-        <v>1856.85</v>
+        <v>1851.65</v>
       </c>
       <c r="K7" t="n">
         <v>4232.74</v>
@@ -1455,10 +1455,10 @@
         <v>10518.1</v>
       </c>
       <c r="M7" t="n">
-        <v>5823.74</v>
+        <v>5818.54</v>
       </c>
       <c r="N7" t="n">
-        <v>4604.47</v>
+        <v>4280.99</v>
       </c>
     </row>
     <row r="8">
@@ -1468,7 +1468,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2071.78</v>
+        <v>2067.51</v>
       </c>
       <c r="C8" t="n">
         <v>4644.47</v>
@@ -1477,7 +1477,7 @@
         <v>4177.12</v>
       </c>
       <c r="E8" t="n">
-        <v>2460.15</v>
+        <v>2459.81</v>
       </c>
       <c r="F8" t="n">
         <v>6076.23</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>7036.33</v>
+        <v>7036.3</v>
       </c>
       <c r="J8" t="n">
         <v>4975.2</v>
@@ -1514,7 +1514,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8034.41</v>
+        <v>8030.14</v>
       </c>
       <c r="C9" t="n">
         <v>10646.29</v>
@@ -1523,13 +1523,13 @@
         <v>10139.75</v>
       </c>
       <c r="E9" t="n">
-        <v>8461.969999999999</v>
+        <v>8461.629999999999</v>
       </c>
       <c r="F9" t="n">
-        <v>11312.91</v>
+        <v>11311.15</v>
       </c>
       <c r="G9" t="n">
-        <v>11317.08</v>
+        <v>11311.46</v>
       </c>
       <c r="H9" t="n">
         <v>6876.56</v>
@@ -1541,13 +1541,13 @@
         <v>10977.02</v>
       </c>
       <c r="K9" t="n">
-        <v>9172.879999999999</v>
+        <v>9171.120000000001</v>
       </c>
       <c r="L9" t="n">
         <v>3609.96</v>
       </c>
       <c r="M9" t="n">
-        <v>13319.33</v>
+        <v>13321.27</v>
       </c>
       <c r="N9" t="n">
         <v>10156.51</v>
@@ -1560,13 +1560,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5401.27</v>
+        <v>5397</v>
       </c>
       <c r="C10" t="n">
         <v>3009.67</v>
       </c>
       <c r="D10" t="n">
-        <v>3886.08</v>
+        <v>3739.54</v>
       </c>
       <c r="E10" t="n">
         <v>3769.54</v>
@@ -1581,13 +1581,13 @@
         <v>5078.06</v>
       </c>
       <c r="I10" t="n">
-        <v>11247.96</v>
+        <v>11247.93</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>4874.27</v>
+        <v>4874.26</v>
       </c>
       <c r="L10" t="n">
         <v>10174.36</v>
@@ -1596,7 +1596,7 @@
         <v>6761.26</v>
       </c>
       <c r="N10" t="n">
-        <v>3536.67</v>
+        <v>3218.39</v>
       </c>
     </row>
     <row r="11">
@@ -1606,13 +1606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5934.68</v>
+        <v>5930.4</v>
       </c>
       <c r="C11" t="n">
         <v>5735.32</v>
       </c>
       <c r="D11" t="n">
-        <v>6506.55</v>
+        <v>6465.19</v>
       </c>
       <c r="E11" t="n">
         <v>4420.85</v>
@@ -1621,7 +1621,7 @@
         <v>4028.53</v>
       </c>
       <c r="G11" t="n">
-        <v>4032.71</v>
+        <v>4028.84</v>
       </c>
       <c r="H11" t="n">
         <v>5264.26</v>
@@ -1630,7 +1630,7 @@
         <v>9238.09</v>
       </c>
       <c r="J11" t="n">
-        <v>4931.45</v>
+        <v>4931.44</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
@@ -1642,7 +1642,7 @@
         <v>6539.69</v>
       </c>
       <c r="N11" t="n">
-        <v>6262.31</v>
+        <v>5944.03</v>
       </c>
     </row>
     <row r="12">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6437.48</v>
+        <v>6433.21</v>
       </c>
       <c r="C12" t="n">
         <v>9144.57</v>
@@ -1661,31 +1661,31 @@
         <v>8506.360000000001</v>
       </c>
       <c r="E12" t="n">
-        <v>7462.7</v>
+        <v>7461.29</v>
       </c>
       <c r="F12" t="n">
-        <v>11002.42</v>
+        <v>11001.36</v>
       </c>
       <c r="G12" t="n">
-        <v>10456.74</v>
+        <v>10455.67</v>
       </c>
       <c r="H12" t="n">
-        <v>5877.28</v>
+        <v>5876.22</v>
       </c>
       <c r="I12" t="n">
-        <v>3743.47</v>
+        <v>3743.44</v>
       </c>
       <c r="J12" t="n">
-        <v>9977.75</v>
+        <v>9976.68</v>
       </c>
       <c r="K12" t="n">
-        <v>8862.389999999999</v>
+        <v>8861.33</v>
       </c>
       <c r="L12" t="n">
         <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>13945.57</v>
+        <v>13944.51</v>
       </c>
       <c r="N12" t="n">
         <v>8523.120000000001</v>
@@ -1698,13 +1698,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9411.09</v>
+        <v>9406.82</v>
       </c>
       <c r="C13" t="n">
-        <v>8701.549999999999</v>
+        <v>8740.139999999999</v>
       </c>
       <c r="D13" t="n">
-        <v>9577.950000000001</v>
+        <v>9470.01</v>
       </c>
       <c r="E13" t="n">
         <v>7779.36</v>
@@ -1719,7 +1719,7 @@
         <v>9095.33</v>
       </c>
       <c r="I13" t="n">
-        <v>13156.39</v>
+        <v>13156.62</v>
       </c>
       <c r="J13" t="n">
         <v>6632.34</v>
@@ -1734,7 +1734,7 @@
         <v>0</v>
       </c>
       <c r="N13" t="n">
-        <v>9228.540000000001</v>
+        <v>8948.85</v>
       </c>
     </row>
     <row r="14">
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>3537.2</v>
+        <v>3532.92</v>
       </c>
       <c r="C14" t="n">
         <v>1066.93</v>
@@ -1765,7 +1765,7 @@
         <v>4152.39</v>
       </c>
       <c r="I14" t="n">
-        <v>10346.36</v>
+        <v>10346.33</v>
       </c>
       <c r="J14" t="n">
         <v>3193.51</v>

</xml_diff>